<commit_message>
Add directions to elec/ETS and set shareweight for two plant types to zero (#125)
</commit_message>
<xml_diff>
--- a/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
+++ b/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\elec\ETS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA71630-DF33-4A18-BE64-C379BE81972A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC39DC9C-4ABD-4985-BBEF-F8A2C75F8398}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24810" yWindow="3630" windowWidth="28560" windowHeight="19110" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="27435" yWindow="3690" windowWidth="28560" windowHeight="19110" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>ETS Electricity Technology Shareweights</t>
   </si>
@@ -106,14 +106,89 @@
     <t>technology selection.  For more on this, see the "Modified Logit" equation description at:</t>
   </si>
   <si>
-    <t>None needed.  Handled through calibration. Done through calibration</t>
+    <t>None</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It is recommended that you base these shareweights on the percentage of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>new</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> electricity</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">demand that could be met by deploying </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>new</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> capacity of each technology in each particular year.</t>
+    </r>
+  </si>
+  <si>
+    <t>"New" electricity demand can come from increased demand (for instance, due to electrification)</t>
+  </si>
+  <si>
+    <t>or from retirements of existing power plants (so some new plant needs to be built to supply the</t>
+  </si>
+  <si>
+    <t>electricity demand have some "new" demand due to plant retirements.  Only a country with</t>
+  </si>
+  <si>
+    <t>electricity demand that is declining at a faster rate than power plant are retiring has no "new"</t>
+  </si>
+  <si>
+    <t>built, so the shareweights chosen here do not matter.)</t>
+  </si>
+  <si>
+    <t>electricity that used to be supplied by the retiring plant).  Therefore, even countries with flat</t>
+  </si>
+  <si>
+    <t>electricity demand for purposes of this variable.  (In this unusual case, no new plants are being</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +214,15 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -487,7 +571,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6422D012-50FD-4D0C-A3BE-19778A6AC198}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -526,11 +610,57 @@
         <v>20</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A8" r:id="rId1" xr:uid="{2705635C-9EE8-4C02-9AF9-24B17956AB3A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1925,97 +2055,97 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
@@ -2023,97 +2153,97 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">

</xml_diff>